<commit_message>
Initialised tables and added data for sizes,elements and ailments tables.
</commit_message>
<xml_diff>
--- a/Resources/Normalisation.xlsx
+++ b/Resources/Normalisation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchan\Documents\Sparta Global\CodeAlong\Assignment\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6D75CA-784F-42B6-8B55-940A22202FF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E62A3C-38BC-4000-B91B-249AA48012EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="1905" windowWidth="21600" windowHeight="11385" xr2:uid="{D64CD4D8-DB5B-4155-B078-1ABA991075A7}"/>
   </bookViews>
@@ -565,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6A4B970-33B5-4197-A1F2-13574CCCED12}">
   <dimension ref="E4:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="27.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" customWidth="1"/>
     <col min="16" max="16" width="24.5703125" bestFit="1" customWidth="1"/>

</xml_diff>